<commit_message>
Added the divider delay time to the metadata files.
Added the divider delay time to the metadata files.
</commit_message>
<xml_diff>
--- a/ledProtocols/protocolRGBTemplate.xlsx
+++ b/ledProtocols/protocolRGBTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\labadmin\Documents\MATLAB\FlyBubbleRGB\ledProtocols\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93AFF8AD-D7E8-4A7B-ADF1-01B0D38281F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40F2315-1A0B-413F-A160-CFF1DE5A2D75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4980" yWindow="1740" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1002,7 +1002,7 @@
   <dimension ref="A1:CF3343"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1321,10 +1321,10 @@
         <v>5</v>
       </c>
       <c r="J6" s="20">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="K6" s="20">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="L6" s="20">
         <v>2000</v>

</xml_diff>